<commit_message>
fixes to BOM - 5/14/2013
</commit_message>
<xml_diff>
--- a/Drumpants_A2_BOM_5-10-2014.xlsx
+++ b/Drumpants_A2_BOM_5-10-2014.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="22050" yWindow="-90" windowWidth="20730" windowHeight="11550"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="BOARD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -476,9 +476,6 @@
     <t>C1, C4, C55</t>
   </si>
   <si>
-    <t>R24, R25, R38</t>
-  </si>
-  <si>
     <t>C2, C8, C9</t>
   </si>
   <si>
@@ -570,16 +567,19 @@
   </si>
   <si>
     <t>R7, R10, R3, R39</t>
+  </si>
+  <si>
+    <t>R24, R25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1346,7 +1346,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1601,7 +1601,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1636,7 +1635,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1812,14 +1810,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
@@ -1834,7 +1832,7 @@
     <col min="11" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1863,7 +1861,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -1893,67 +1891,67 @@
       </c>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="I3" s="1">
         <v>3000</v>
       </c>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="I4" s="1">
         <v>3000</v>
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1983,7 +1981,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="13" t="s">
         <v>141</v>
       </c>
@@ -2013,9 +2011,9 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>11</v>
@@ -2043,7 +2041,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
@@ -2073,7 +2071,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="16" customFormat="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
@@ -2096,9 +2094,9 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="16" customFormat="1">
       <c r="A10" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>9</v>
@@ -2119,7 +2117,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="16" customFormat="1">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
@@ -2141,7 +2139,7 @@
       <c r="G11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="16" customFormat="1">
       <c r="A12" s="13" t="s">
         <v>23</v>
       </c>
@@ -2164,7 +2162,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:10" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -2187,7 +2185,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="16" customFormat="1">
       <c r="A14" s="13" t="s">
         <v>24</v>
       </c>
@@ -2210,7 +2208,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="16" customFormat="1">
       <c r="A15" s="13" t="s">
         <v>139</v>
       </c>
@@ -2233,9 +2231,9 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="16" customFormat="1">
       <c r="A16" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>93</v>
@@ -2244,10 +2242,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>155</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>156</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>85</v>
@@ -2256,27 +2254,27 @@
         <v>94</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I16" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="16" customFormat="1">
       <c r="A17" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>85</v>
@@ -2285,13 +2283,13 @@
         <v>124</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I17" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="11" t="s">
         <v>26</v>
       </c>
@@ -2321,7 +2319,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="11" t="s">
         <v>127</v>
       </c>
@@ -2332,10 +2330,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>85</v>
@@ -2344,19 +2342,19 @@
         <v>124</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>126</v>
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -2371,7 +2369,7 @@
         <v>85</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H20" s="3">
         <v>532610371</v>
@@ -2381,12 +2379,12 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -2411,7 +2409,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="11" t="s">
         <v>31</v>
       </c>
@@ -2441,12 +2439,12 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -2471,7 +2469,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="11" t="s">
         <v>35</v>
       </c>
@@ -2501,7 +2499,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="11" t="s">
         <v>37</v>
       </c>
@@ -2531,7 +2529,7 @@
       </c>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="13" t="s">
         <v>39</v>
       </c>
@@ -2555,7 +2553,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="13" t="s">
         <v>45</v>
       </c>
@@ -2579,7 +2577,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="13" t="s">
         <v>48</v>
       </c>
@@ -2603,7 +2601,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="13" t="s">
         <v>49</v>
       </c>
@@ -2627,7 +2625,7 @@
       <c r="I29" s="14"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="13" t="s">
         <v>140</v>
       </c>
@@ -2651,15 +2649,15 @@
       <c r="I30" s="14"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:10" s="16" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="16" customFormat="1" ht="13.9" customHeight="1">
       <c r="A31" s="13" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>50</v>
@@ -2674,7 +2672,7 @@
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="16" customFormat="1">
       <c r="A32" s="13" t="s">
         <v>51</v>
       </c>
@@ -2697,7 +2695,7 @@
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="16" customFormat="1">
       <c r="A33" s="13" t="s">
         <v>53</v>
       </c>
@@ -2720,7 +2718,7 @@
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="16" customFormat="1">
       <c r="A34" s="13" t="s">
         <v>42</v>
       </c>
@@ -2743,9 +2741,9 @@
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="16" customFormat="1">
       <c r="A35" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>41</v>
@@ -2766,7 +2764,7 @@
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="16" customFormat="1">
       <c r="A36" s="13" t="s">
         <v>43</v>
       </c>
@@ -2789,7 +2787,7 @@
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="16" customFormat="1">
       <c r="A37" s="11" t="s">
         <v>54</v>
       </c>
@@ -2800,10 +2798,10 @@
         <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>104</v>
@@ -2818,7 +2816,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="16" customFormat="1">
       <c r="A38" s="11" t="s">
         <v>55</v>
       </c>
@@ -2847,7 +2845,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="16" customFormat="1">
       <c r="A39" s="11" t="s">
         <v>58</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="16" customFormat="1">
       <c r="A40" s="11" t="s">
         <v>61</v>
       </c>
@@ -2905,7 +2903,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="16" customFormat="1">
       <c r="A41" s="11" t="s">
         <v>63</v>
       </c>
@@ -2934,7 +2932,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="11" t="s">
         <v>66</v>
       </c>
@@ -2964,7 +2962,7 @@
       </c>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="11" t="s">
         <v>69</v>
       </c>
@@ -2994,21 +2992,21 @@
       </c>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>85</v>
@@ -3017,14 +3015,14 @@
         <v>113</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I44" s="1">
         <v>3000</v>
       </c>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="11" t="s">
         <v>72</v>
       </c>
@@ -3054,7 +3052,7 @@
       </c>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="11" t="s">
         <v>74</v>
       </c>
@@ -3084,7 +3082,7 @@
       </c>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="11" t="s">
         <v>77</v>
       </c>
@@ -3114,7 +3112,7 @@
       </c>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="11" t="s">
         <v>80</v>
       </c>

</xml_diff>